<commit_message>
Genetic + Local Search
</commit_message>
<xml_diff>
--- a/GraphPartitionTODOs.xlsx
+++ b/GraphPartitionTODOs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuval\Desktop\GraphPartition\GraphPartition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7206E02-8A55-4E4D-84F3-BF562439CFCC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F88D5D-11F7-49C9-AB41-121EC41263D8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="3" xr2:uid="{F0443E2F-E498-43DC-84E2-B84720F00A32}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="4" xr2:uid="{F0443E2F-E498-43DC-84E2-B84720F00A32}"/>
   </bookViews>
   <sheets>
     <sheet name="Graphs" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Local Search" sheetId="3" r:id="rId3"/>
     <sheet name="Branch &amp; Bound" sheetId="4" r:id="rId4"/>
     <sheet name="Analyzation" sheetId="8" r:id="rId5"/>
+    <sheet name="TODOs" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="106">
   <si>
     <t>Graphs</t>
   </si>
@@ -175,12 +176,6 @@
     <t>Running Time</t>
   </si>
   <si>
-    <t>Min-Bound Analyzation</t>
-  </si>
-  <si>
-    <t>Random vs Greedy  Upper Bound Analyzation</t>
-  </si>
-  <si>
     <t>Upper Bound</t>
   </si>
   <si>
@@ -308,6 +303,51 @@
   </si>
   <si>
     <t>Copy One Partition</t>
+  </si>
+  <si>
+    <t>2.5^#Nodes</t>
+  </si>
+  <si>
+    <t>1.5 hours</t>
+  </si>
+  <si>
+    <t>3.1 hours</t>
+  </si>
+  <si>
+    <t>5.3 hours</t>
+  </si>
+  <si>
+    <t>2.2 hours</t>
+  </si>
+  <si>
+    <t>Even Graph</t>
+  </si>
+  <si>
+    <t>Min-Bound Analysis</t>
+  </si>
+  <si>
+    <t>Random vs Greedy  Upper Bound Analysis</t>
+  </si>
+  <si>
+    <t>Local Search 4 clique 140 nodes, 2 days one swap</t>
+  </si>
+  <si>
+    <t>Branch &amp; Bound:</t>
+  </si>
+  <si>
+    <t>2 Groups, N/2 N/2</t>
+  </si>
+  <si>
+    <t>על כל שיטה</t>
+  </si>
+  <si>
+    <t>תיאור במסמך</t>
+  </si>
+  <si>
+    <t>דוגמאות ריצה - קלטים ופלטים לא ענקיים</t>
+  </si>
+  <si>
+    <t>בין חמישה לעשרה</t>
   </si>
 </sst>
 </file>
@@ -362,7 +402,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="28">
+  <fills count="29">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -525,6 +565,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="54">
     <border>
@@ -1168,19 +1214,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1213,17 +1246,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -1262,6 +1284,34 @@
       </left>
       <right style="thin">
         <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom style="medium">
@@ -1273,7 +1323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1431,24 +1481,6 @@
     <xf numFmtId="0" fontId="4" fillId="15" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1467,37 +1499,76 @@
     <xf numFmtId="0" fontId="0" fillId="25" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1548,85 +1619,25 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1638,6 +1649,69 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="18" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1656,14 +1730,14 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1683,7 +1757,7 @@
     <xf numFmtId="0" fontId="5" fillId="21" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2001,6 +2075,107 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>2.5^#Nodes</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="tx2">
+                    <a:lumMod val="40000"/>
+                    <a:lumOff val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Analyzation!$E$77:$E$81</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Analyzation!$I$77:$I$81</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>39.0625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1525.87890625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>59604.644775390625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2328306.4365386963</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90949470.177292824</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B854-45CA-920C-6EAEE65FCA88}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -2141,11 +2316,15 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:legendEntry>
-        <c:idx val="2"/>
+        <c:idx val="3"/>
         <c:delete val="1"/>
       </c:legendEntry>
       <c:legendEntry>
-        <c:idx val="3"/>
+        <c:idx val="4"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="5"/>
         <c:delete val="1"/>
       </c:legendEntry>
       <c:overlay val="0"/>
@@ -2343,7 +2522,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Analyzation!$E$82:$E$86</c:f>
+              <c:f>Analyzation!$E$88:$E$92</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2367,7 +2546,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Analyzation!$I$82:$I$86</c:f>
+              <c:f>Analyzation!$I$88:$I$92</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2442,7 +2621,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Analyzation!$E$87:$E$91</c:f>
+              <c:f>Analyzation!$E$93:$E$97</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2466,7 +2645,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Analyzation!$I$87:$I$91</c:f>
+              <c:f>Analyzation!$I$93:$I$97</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3821,16 +4000,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>173936</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>33133</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>447262</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>248479</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>24849</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>306456</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>8284</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3859,13 +4038,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>80</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>74543</xdr:colOff>
-      <xdr:row>94</xdr:row>
+      <xdr:row>100</xdr:row>
       <xdr:rowOff>82825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4196,10 +4375,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="B1:C10"/>
+  <dimension ref="B1:C11"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4209,10 +4388,10 @@
   <sheetData>
     <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:3" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="77"/>
+      <c r="C2" s="84"/>
     </row>
     <row r="3" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4257,17 +4436,25 @@
     </row>
     <row r="9" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B9" s="24" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="C9" s="25" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="26" t="s">
+    <row r="10" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="B10" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C11" s="27" t="s">
         <v>8</v>
       </c>
     </row>
@@ -4288,7 +4475,7 @@
   <dimension ref="B1:D20"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:C20"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4298,11 +4485,11 @@
   <sheetData>
     <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:4" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="80"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="87"/>
     </row>
     <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4353,7 +4540,7 @@
       </c>
     </row>
     <row r="9" spans="2:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="B9" s="81" t="s">
+      <c r="B9" s="88" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="13" t="s">
@@ -4364,7 +4551,7 @@
       </c>
     </row>
     <row r="10" spans="2:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="B10" s="81"/>
+      <c r="B10" s="88"/>
       <c r="C10" s="13" t="s">
         <v>17</v>
       </c>
@@ -4373,7 +4560,7 @@
       </c>
     </row>
     <row r="11" spans="2:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="B11" s="81" t="s">
+      <c r="B11" s="88" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="13" t="s">
@@ -4384,7 +4571,7 @@
       </c>
     </row>
     <row r="12" spans="2:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="B12" s="81"/>
+      <c r="B12" s="88"/>
       <c r="C12" s="13" t="s">
         <v>20</v>
       </c>
@@ -4393,7 +4580,7 @@
       </c>
     </row>
     <row r="13" spans="2:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="B13" s="81"/>
+      <c r="B13" s="88"/>
       <c r="C13" s="13" t="s">
         <v>21</v>
       </c>
@@ -4402,7 +4589,7 @@
       </c>
     </row>
     <row r="14" spans="2:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="B14" s="81" t="s">
+      <c r="B14" s="88" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="13" t="s">
@@ -4413,7 +4600,7 @@
       </c>
     </row>
     <row r="15" spans="2:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="B15" s="81"/>
+      <c r="B15" s="88"/>
       <c r="C15" s="13" t="s">
         <v>26</v>
       </c>
@@ -4422,7 +4609,7 @@
       </c>
     </row>
     <row r="16" spans="2:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="B16" s="81"/>
+      <c r="B16" s="88"/>
       <c r="C16" s="13" t="s">
         <v>24</v>
       </c>
@@ -4431,7 +4618,7 @@
       </c>
     </row>
     <row r="17" spans="2:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="B17" s="81"/>
+      <c r="B17" s="88"/>
       <c r="C17" s="13" t="s">
         <v>25</v>
       </c>
@@ -4440,7 +4627,7 @@
       </c>
     </row>
     <row r="18" spans="2:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="B18" s="81"/>
+      <c r="B18" s="88"/>
       <c r="C18" s="13" t="s">
         <v>27</v>
       </c>
@@ -4449,7 +4636,7 @@
       </c>
     </row>
     <row r="19" spans="2:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="B19" s="81"/>
+      <c r="B19" s="88"/>
       <c r="C19" s="13" t="s">
         <v>28</v>
       </c>
@@ -4458,7 +4645,7 @@
       </c>
     </row>
     <row r="20" spans="2:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="82"/>
+      <c r="B20" s="89"/>
       <c r="C20" s="16" t="s">
         <v>29</v>
       </c>
@@ -4485,7 +4672,7 @@
   <dimension ref="B1:D9"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4495,11 +4682,11 @@
   <sheetData>
     <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:4" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="90" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="85"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="92"/>
     </row>
     <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4523,7 +4710,7 @@
       </c>
     </row>
     <row r="6" spans="2:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="B6" s="86" t="s">
+      <c r="B6" s="93" t="s">
         <v>33</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -4534,7 +4721,7 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="B7" s="86"/>
+      <c r="B7" s="93"/>
       <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
@@ -4543,7 +4730,7 @@
       </c>
     </row>
     <row r="8" spans="2:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="B8" s="87"/>
+      <c r="B8" s="94"/>
       <c r="C8" s="32" t="s">
         <v>21</v>
       </c>
@@ -4552,7 +4739,7 @@
       </c>
     </row>
     <row r="9" spans="2:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="88"/>
+      <c r="B9" s="95"/>
       <c r="C9" s="3" t="s">
         <v>38</v>
       </c>
@@ -4576,8 +4763,8 @@
   </sheetPr>
   <dimension ref="B1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4587,11 +4774,11 @@
   <sheetData>
     <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:4" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="96" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="91"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="98"/>
     </row>
     <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4606,7 +4793,7 @@
       </c>
     </row>
     <row r="5" spans="2:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="B5" s="93" t="s">
+      <c r="B5" s="99" t="s">
         <v>34</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -4617,7 +4804,7 @@
       </c>
     </row>
     <row r="6" spans="2:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="B6" s="92"/>
+      <c r="B6" s="100"/>
       <c r="C6" s="5" t="s">
         <v>39</v>
       </c>
@@ -4626,7 +4813,7 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="137" t="s">
+      <c r="B7" s="69" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="39" t="s">
@@ -4650,10 +4837,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC1FF"/>
   </sheetPr>
-  <dimension ref="B1:L91"/>
+  <dimension ref="B1:L97"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4672,557 +4859,579 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="134" t="s">
+      <c r="B2" s="142" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="135"/>
-      <c r="D2" s="135"/>
-      <c r="E2" s="135"/>
-      <c r="F2" s="135"/>
-      <c r="G2" s="135"/>
-      <c r="H2" s="135"/>
-      <c r="I2" s="135"/>
-      <c r="J2" s="135"/>
-      <c r="K2" s="135"/>
-      <c r="L2" s="136"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="143"/>
+      <c r="G2" s="143"/>
+      <c r="H2" s="143"/>
+      <c r="I2" s="143"/>
+      <c r="J2" s="143"/>
+      <c r="K2" s="143"/>
+      <c r="L2" s="144"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D4" s="131" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="132"/>
-      <c r="F4" s="132"/>
-      <c r="G4" s="132"/>
-      <c r="H4" s="132"/>
-      <c r="I4" s="132"/>
-      <c r="J4" s="133"/>
+      <c r="D4" s="139" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="140"/>
+      <c r="F4" s="140"/>
+      <c r="G4" s="140"/>
+      <c r="H4" s="140"/>
+      <c r="I4" s="140"/>
+      <c r="J4" s="141"/>
     </row>
     <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="54" t="s">
+      <c r="D6" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="54" t="s">
+      <c r="E6" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="54" t="s">
+      <c r="F6" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="54" t="s">
+      <c r="G6" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="54" t="s">
+      <c r="H6" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="54" t="s">
+      <c r="I6" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="54" t="s">
+      <c r="J6" s="78" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="54" t="s">
+      <c r="K6" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="L6" s="55" t="s">
-        <v>53</v>
+      <c r="L6" s="79" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="104" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" s="100" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" s="100">
+      <c r="B7" s="115" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="103" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="103">
         <v>80</v>
       </c>
-      <c r="E7" s="58">
+      <c r="E7" s="80">
         <v>5</v>
       </c>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="58"/>
-      <c r="K7" s="58"/>
-      <c r="L7" s="74"/>
+      <c r="F7" s="103">
+        <v>0.3</v>
+      </c>
+      <c r="G7" s="103">
+        <v>0.1</v>
+      </c>
+      <c r="H7" s="103">
+        <v>0.05</v>
+      </c>
+      <c r="I7" s="103" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="103" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="103" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" s="68"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="105"/>
-      <c r="C8" s="101"/>
-      <c r="D8" s="101"/>
-      <c r="E8" s="56">
+      <c r="B8" s="116"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="104"/>
+      <c r="E8" s="81">
         <v>10</v>
       </c>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="56"/>
-      <c r="J8" s="56"/>
-      <c r="K8" s="56"/>
-      <c r="L8" s="68"/>
+      <c r="F8" s="104"/>
+      <c r="G8" s="104"/>
+      <c r="H8" s="104"/>
+      <c r="I8" s="104"/>
+      <c r="J8" s="104"/>
+      <c r="K8" s="104"/>
+      <c r="L8" s="62"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="105"/>
-      <c r="C9" s="101"/>
-      <c r="D9" s="101"/>
-      <c r="E9" s="56">
+      <c r="B9" s="116"/>
+      <c r="C9" s="104"/>
+      <c r="D9" s="104"/>
+      <c r="E9" s="81">
         <v>20</v>
       </c>
-      <c r="F9" s="56"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="56"/>
-      <c r="K9" s="56"/>
-      <c r="L9" s="68"/>
+      <c r="F9" s="104"/>
+      <c r="G9" s="104"/>
+      <c r="H9" s="104"/>
+      <c r="I9" s="104"/>
+      <c r="J9" s="104"/>
+      <c r="K9" s="104"/>
+      <c r="L9" s="62"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="105"/>
-      <c r="C10" s="101"/>
-      <c r="D10" s="101"/>
-      <c r="E10" s="56">
+      <c r="B10" s="116"/>
+      <c r="C10" s="104"/>
+      <c r="D10" s="104"/>
+      <c r="E10" s="81">
         <v>40</v>
       </c>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="56"/>
-      <c r="L10" s="68"/>
+      <c r="F10" s="104"/>
+      <c r="G10" s="104"/>
+      <c r="H10" s="104"/>
+      <c r="I10" s="104"/>
+      <c r="J10" s="104"/>
+      <c r="K10" s="104"/>
+      <c r="L10" s="62"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="105"/>
-      <c r="C11" s="101"/>
-      <c r="D11" s="101"/>
-      <c r="E11" s="75">
+      <c r="B11" s="116"/>
+      <c r="C11" s="104"/>
+      <c r="D11" s="104"/>
+      <c r="E11" s="81">
         <v>60</v>
       </c>
-      <c r="F11" s="56"/>
-      <c r="G11" s="56"/>
-      <c r="H11" s="56"/>
-      <c r="I11" s="56"/>
-      <c r="J11" s="56"/>
-      <c r="K11" s="56"/>
-      <c r="L11" s="68"/>
+      <c r="F11" s="104"/>
+      <c r="G11" s="104"/>
+      <c r="H11" s="104"/>
+      <c r="I11" s="104"/>
+      <c r="J11" s="104"/>
+      <c r="K11" s="104"/>
+      <c r="L11" s="62"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="105"/>
-      <c r="C12" s="101"/>
-      <c r="D12" s="101"/>
-      <c r="E12" s="103">
+      <c r="B12" s="116"/>
+      <c r="C12" s="104"/>
+      <c r="D12" s="104"/>
+      <c r="E12" s="104">
         <v>20</v>
       </c>
-      <c r="F12" s="56">
+      <c r="F12" s="81">
         <v>0.2</v>
       </c>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="56"/>
-      <c r="L12" s="68"/>
+      <c r="G12" s="104"/>
+      <c r="H12" s="104"/>
+      <c r="I12" s="104"/>
+      <c r="J12" s="104"/>
+      <c r="K12" s="104"/>
+      <c r="L12" s="62"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="105"/>
-      <c r="C13" s="101"/>
-      <c r="D13" s="101"/>
-      <c r="E13" s="101"/>
-      <c r="F13" s="56">
+      <c r="B13" s="116"/>
+      <c r="C13" s="104"/>
+      <c r="D13" s="104"/>
+      <c r="E13" s="104"/>
+      <c r="F13" s="81">
         <v>0.4</v>
       </c>
-      <c r="G13" s="56"/>
-      <c r="H13" s="56"/>
-      <c r="I13" s="56"/>
-      <c r="J13" s="56"/>
-      <c r="K13" s="56"/>
-      <c r="L13" s="68"/>
+      <c r="G13" s="104"/>
+      <c r="H13" s="104"/>
+      <c r="I13" s="104"/>
+      <c r="J13" s="104"/>
+      <c r="K13" s="104"/>
+      <c r="L13" s="62"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="105"/>
-      <c r="C14" s="101"/>
-      <c r="D14" s="101"/>
-      <c r="E14" s="101"/>
-      <c r="F14" s="56">
+      <c r="B14" s="116"/>
+      <c r="C14" s="104"/>
+      <c r="D14" s="104"/>
+      <c r="E14" s="104"/>
+      <c r="F14" s="81">
         <v>0.6</v>
       </c>
-      <c r="G14" s="56"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="56"/>
-      <c r="L14" s="68"/>
+      <c r="G14" s="104"/>
+      <c r="H14" s="104"/>
+      <c r="I14" s="104"/>
+      <c r="J14" s="104"/>
+      <c r="K14" s="104"/>
+      <c r="L14" s="62"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="105"/>
-      <c r="C15" s="101"/>
-      <c r="D15" s="101"/>
-      <c r="E15" s="101"/>
-      <c r="F15" s="56">
+      <c r="B15" s="116"/>
+      <c r="C15" s="104"/>
+      <c r="D15" s="104"/>
+      <c r="E15" s="104"/>
+      <c r="F15" s="81">
         <v>0.8</v>
       </c>
-      <c r="G15" s="56"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="56"/>
-      <c r="K15" s="56"/>
-      <c r="L15" s="68"/>
+      <c r="G15" s="104"/>
+      <c r="H15" s="104"/>
+      <c r="I15" s="104"/>
+      <c r="J15" s="104"/>
+      <c r="K15" s="104"/>
+      <c r="L15" s="62"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="105"/>
-      <c r="C16" s="101"/>
-      <c r="D16" s="101"/>
-      <c r="E16" s="101"/>
-      <c r="F16" s="56">
+      <c r="B16" s="116"/>
+      <c r="C16" s="104"/>
+      <c r="D16" s="104"/>
+      <c r="E16" s="104"/>
+      <c r="F16" s="81">
         <v>1</v>
       </c>
-      <c r="G16" s="56"/>
-      <c r="H16" s="56"/>
-      <c r="I16" s="56"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="56"/>
-      <c r="L16" s="68"/>
+      <c r="G16" s="104"/>
+      <c r="H16" s="104"/>
+      <c r="I16" s="104"/>
+      <c r="J16" s="104"/>
+      <c r="K16" s="104"/>
+      <c r="L16" s="62"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="105"/>
-      <c r="C17" s="101"/>
-      <c r="D17" s="101"/>
-      <c r="E17" s="101"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="56">
+      <c r="B17" s="116"/>
+      <c r="C17" s="104"/>
+      <c r="D17" s="104"/>
+      <c r="E17" s="104"/>
+      <c r="F17" s="104">
+        <v>0.3</v>
+      </c>
+      <c r="G17" s="81">
         <v>0.1</v>
       </c>
-      <c r="H17" s="56"/>
-      <c r="I17" s="56"/>
-      <c r="J17" s="56"/>
-      <c r="K17" s="56"/>
-      <c r="L17" s="68"/>
+      <c r="H17" s="104"/>
+      <c r="I17" s="104"/>
+      <c r="J17" s="104"/>
+      <c r="K17" s="104"/>
+      <c r="L17" s="62"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="105"/>
-      <c r="C18" s="101"/>
-      <c r="D18" s="101"/>
-      <c r="E18" s="101"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56">
+      <c r="B18" s="116"/>
+      <c r="C18" s="104"/>
+      <c r="D18" s="104"/>
+      <c r="E18" s="104"/>
+      <c r="F18" s="104"/>
+      <c r="G18" s="81">
         <v>0.2</v>
       </c>
-      <c r="H18" s="56"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="56"/>
-      <c r="K18" s="56"/>
-      <c r="L18" s="68"/>
+      <c r="H18" s="104"/>
+      <c r="I18" s="104"/>
+      <c r="J18" s="104"/>
+      <c r="K18" s="104"/>
+      <c r="L18" s="62"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="105"/>
-      <c r="C19" s="101"/>
-      <c r="D19" s="101"/>
-      <c r="E19" s="101"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="56">
+      <c r="B19" s="116"/>
+      <c r="C19" s="104"/>
+      <c r="D19" s="104"/>
+      <c r="E19" s="104"/>
+      <c r="F19" s="104"/>
+      <c r="G19" s="81">
         <v>0.4</v>
       </c>
-      <c r="H19" s="56"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
-      <c r="K19" s="56"/>
-      <c r="L19" s="68"/>
+      <c r="H19" s="104"/>
+      <c r="I19" s="104"/>
+      <c r="J19" s="104"/>
+      <c r="K19" s="104"/>
+      <c r="L19" s="62"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="105"/>
-      <c r="C20" s="101"/>
-      <c r="D20" s="101"/>
-      <c r="E20" s="101"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="56">
+      <c r="B20" s="116"/>
+      <c r="C20" s="104"/>
+      <c r="D20" s="104"/>
+      <c r="E20" s="104"/>
+      <c r="F20" s="104"/>
+      <c r="G20" s="81">
         <v>0.6</v>
       </c>
-      <c r="H20" s="56"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="56"/>
-      <c r="K20" s="56"/>
-      <c r="L20" s="68"/>
+      <c r="H20" s="104"/>
+      <c r="I20" s="104"/>
+      <c r="J20" s="104"/>
+      <c r="K20" s="104"/>
+      <c r="L20" s="62"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="105"/>
-      <c r="C21" s="101"/>
-      <c r="D21" s="101"/>
-      <c r="E21" s="101"/>
-      <c r="F21" s="56"/>
-      <c r="G21" s="56"/>
-      <c r="H21" s="56">
+      <c r="B21" s="116"/>
+      <c r="C21" s="104"/>
+      <c r="D21" s="104"/>
+      <c r="E21" s="104"/>
+      <c r="F21" s="104"/>
+      <c r="G21" s="104">
+        <v>0.1</v>
+      </c>
+      <c r="H21" s="81">
         <v>0.05</v>
       </c>
-      <c r="I21" s="56"/>
-      <c r="J21" s="56"/>
-      <c r="K21" s="56"/>
-      <c r="L21" s="68"/>
+      <c r="I21" s="104"/>
+      <c r="J21" s="104"/>
+      <c r="K21" s="104"/>
+      <c r="L21" s="62"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="105"/>
-      <c r="C22" s="101"/>
-      <c r="D22" s="101"/>
-      <c r="E22" s="101"/>
-      <c r="F22" s="56"/>
-      <c r="G22" s="56"/>
-      <c r="H22" s="56">
+      <c r="B22" s="116"/>
+      <c r="C22" s="104"/>
+      <c r="D22" s="104"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="104"/>
+      <c r="G22" s="104"/>
+      <c r="H22" s="81">
         <v>0.1</v>
       </c>
-      <c r="I22" s="56"/>
-      <c r="J22" s="56"/>
-      <c r="K22" s="56"/>
-      <c r="L22" s="68"/>
+      <c r="I22" s="104"/>
+      <c r="J22" s="104"/>
+      <c r="K22" s="104"/>
+      <c r="L22" s="62"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="105"/>
-      <c r="C23" s="101"/>
-      <c r="D23" s="101"/>
-      <c r="E23" s="101"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="56"/>
-      <c r="H23" s="56">
+      <c r="B23" s="116"/>
+      <c r="C23" s="104"/>
+      <c r="D23" s="104"/>
+      <c r="E23" s="104"/>
+      <c r="F23" s="104"/>
+      <c r="G23" s="104"/>
+      <c r="H23" s="81">
         <v>0.2</v>
       </c>
-      <c r="I23" s="56"/>
-      <c r="J23" s="56"/>
-      <c r="K23" s="56"/>
-      <c r="L23" s="68"/>
+      <c r="I23" s="104"/>
+      <c r="J23" s="104"/>
+      <c r="K23" s="104"/>
+      <c r="L23" s="62"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="105"/>
-      <c r="C24" s="101"/>
-      <c r="D24" s="101"/>
-      <c r="E24" s="101"/>
-      <c r="F24" s="56"/>
-      <c r="G24" s="56"/>
-      <c r="H24" s="56">
+      <c r="B24" s="116"/>
+      <c r="C24" s="104"/>
+      <c r="D24" s="104"/>
+      <c r="E24" s="104"/>
+      <c r="F24" s="104"/>
+      <c r="G24" s="104"/>
+      <c r="H24" s="81">
         <v>0.4</v>
       </c>
-      <c r="I24" s="56"/>
-      <c r="J24" s="56"/>
-      <c r="K24" s="56"/>
-      <c r="L24" s="68"/>
+      <c r="I24" s="104"/>
+      <c r="J24" s="104"/>
+      <c r="K24" s="104"/>
+      <c r="L24" s="62"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="105"/>
-      <c r="C25" s="101"/>
-      <c r="D25" s="101"/>
-      <c r="E25" s="101"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="56"/>
-      <c r="H25" s="56"/>
-      <c r="I25" s="56" t="s">
+      <c r="B25" s="116"/>
+      <c r="C25" s="104"/>
+      <c r="D25" s="104"/>
+      <c r="E25" s="104"/>
+      <c r="F25" s="104"/>
+      <c r="G25" s="104"/>
+      <c r="H25" s="104">
+        <v>0.05</v>
+      </c>
+      <c r="I25" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="J25" s="56"/>
-      <c r="K25" s="56"/>
-      <c r="L25" s="68"/>
+      <c r="J25" s="104"/>
+      <c r="K25" s="104"/>
+      <c r="L25" s="62"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="105"/>
-      <c r="C26" s="101"/>
-      <c r="D26" s="101"/>
-      <c r="E26" s="101"/>
-      <c r="F26" s="56"/>
-      <c r="G26" s="56"/>
-      <c r="H26" s="56"/>
-      <c r="I26" s="56" t="s">
-        <v>92</v>
-      </c>
-      <c r="J26" s="56"/>
-      <c r="K26" s="56"/>
-      <c r="L26" s="68"/>
+      <c r="B26" s="116"/>
+      <c r="C26" s="104"/>
+      <c r="D26" s="104"/>
+      <c r="E26" s="104"/>
+      <c r="F26" s="104"/>
+      <c r="G26" s="104"/>
+      <c r="H26" s="104"/>
+      <c r="I26" s="81" t="s">
+        <v>90</v>
+      </c>
+      <c r="J26" s="104"/>
+      <c r="K26" s="104"/>
+      <c r="L26" s="62"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="105"/>
-      <c r="C27" s="101"/>
-      <c r="D27" s="101"/>
-      <c r="E27" s="101"/>
-      <c r="F27" s="56"/>
-      <c r="G27" s="56"/>
-      <c r="H27" s="56"/>
-      <c r="I27" s="56"/>
-      <c r="J27" s="56" t="s">
+      <c r="B27" s="116"/>
+      <c r="C27" s="104"/>
+      <c r="D27" s="104"/>
+      <c r="E27" s="104"/>
+      <c r="F27" s="104"/>
+      <c r="G27" s="104"/>
+      <c r="H27" s="104"/>
+      <c r="I27" s="104" t="s">
+        <v>16</v>
+      </c>
+      <c r="J27" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="K27" s="56"/>
-      <c r="L27" s="68"/>
+      <c r="K27" s="104"/>
+      <c r="L27" s="62"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="105"/>
-      <c r="C28" s="101"/>
-      <c r="D28" s="101"/>
-      <c r="E28" s="101"/>
-      <c r="F28" s="56"/>
-      <c r="G28" s="56"/>
-      <c r="H28" s="56"/>
-      <c r="I28" s="56"/>
-      <c r="J28" s="56" t="s">
+      <c r="B28" s="116"/>
+      <c r="C28" s="104"/>
+      <c r="D28" s="104"/>
+      <c r="E28" s="104"/>
+      <c r="F28" s="104"/>
+      <c r="G28" s="104"/>
+      <c r="H28" s="104"/>
+      <c r="I28" s="104"/>
+      <c r="J28" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="K28" s="56"/>
-      <c r="L28" s="68"/>
+      <c r="K28" s="104"/>
+      <c r="L28" s="62"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="105"/>
-      <c r="C29" s="101"/>
-      <c r="D29" s="101"/>
-      <c r="E29" s="101"/>
-      <c r="F29" s="56"/>
-      <c r="G29" s="56"/>
-      <c r="H29" s="56"/>
-      <c r="I29" s="56"/>
-      <c r="J29" s="56" t="s">
+      <c r="B29" s="116"/>
+      <c r="C29" s="104"/>
+      <c r="D29" s="104"/>
+      <c r="E29" s="104"/>
+      <c r="F29" s="104"/>
+      <c r="G29" s="104"/>
+      <c r="H29" s="104"/>
+      <c r="I29" s="104"/>
+      <c r="J29" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="K29" s="56"/>
-      <c r="L29" s="68"/>
+      <c r="K29" s="104"/>
+      <c r="L29" s="62"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B30" s="105"/>
-      <c r="C30" s="101"/>
-      <c r="D30" s="101"/>
-      <c r="E30" s="101"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="56"/>
-      <c r="I30" s="56"/>
-      <c r="J30" s="56"/>
-      <c r="K30" s="56" t="s">
+      <c r="B30" s="116"/>
+      <c r="C30" s="104"/>
+      <c r="D30" s="104"/>
+      <c r="E30" s="104"/>
+      <c r="F30" s="104"/>
+      <c r="G30" s="104"/>
+      <c r="H30" s="104"/>
+      <c r="I30" s="104"/>
+      <c r="J30" s="104" t="s">
+        <v>19</v>
+      </c>
+      <c r="K30" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="L30" s="68"/>
+      <c r="L30" s="62"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B31" s="105"/>
-      <c r="C31" s="101"/>
-      <c r="D31" s="101"/>
-      <c r="E31" s="101"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="56"/>
-      <c r="K31" s="56" t="s">
+      <c r="B31" s="116"/>
+      <c r="C31" s="104"/>
+      <c r="D31" s="104"/>
+      <c r="E31" s="104"/>
+      <c r="F31" s="104"/>
+      <c r="G31" s="104"/>
+      <c r="H31" s="104"/>
+      <c r="I31" s="104"/>
+      <c r="J31" s="104"/>
+      <c r="K31" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="L31" s="68"/>
+      <c r="L31" s="62"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B32" s="105"/>
-      <c r="C32" s="101"/>
-      <c r="D32" s="101"/>
-      <c r="E32" s="101"/>
-      <c r="F32" s="56"/>
-      <c r="G32" s="56"/>
-      <c r="H32" s="56"/>
-      <c r="I32" s="56"/>
-      <c r="J32" s="56"/>
-      <c r="K32" s="56" t="s">
+      <c r="B32" s="116"/>
+      <c r="C32" s="104"/>
+      <c r="D32" s="104"/>
+      <c r="E32" s="104"/>
+      <c r="F32" s="104"/>
+      <c r="G32" s="104"/>
+      <c r="H32" s="104"/>
+      <c r="I32" s="104"/>
+      <c r="J32" s="104"/>
+      <c r="K32" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="L32" s="68"/>
+      <c r="L32" s="62"/>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B33" s="105"/>
-      <c r="C33" s="101"/>
-      <c r="D33" s="101"/>
-      <c r="E33" s="101"/>
-      <c r="F33" s="56"/>
-      <c r="G33" s="56"/>
-      <c r="H33" s="56"/>
-      <c r="I33" s="56"/>
-      <c r="J33" s="56"/>
-      <c r="K33" s="56" t="s">
+      <c r="B33" s="116"/>
+      <c r="C33" s="104"/>
+      <c r="D33" s="104"/>
+      <c r="E33" s="104"/>
+      <c r="F33" s="104"/>
+      <c r="G33" s="104"/>
+      <c r="H33" s="104"/>
+      <c r="I33" s="104"/>
+      <c r="J33" s="104"/>
+      <c r="K33" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="L33" s="68"/>
+      <c r="L33" s="62"/>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B34" s="105"/>
-      <c r="C34" s="101"/>
-      <c r="D34" s="101"/>
-      <c r="E34" s="101"/>
-      <c r="F34" s="56"/>
-      <c r="G34" s="56"/>
-      <c r="H34" s="56"/>
-      <c r="I34" s="56"/>
-      <c r="J34" s="56"/>
-      <c r="K34" s="56" t="s">
+      <c r="B34" s="116"/>
+      <c r="C34" s="104"/>
+      <c r="D34" s="104"/>
+      <c r="E34" s="104"/>
+      <c r="F34" s="104"/>
+      <c r="G34" s="104"/>
+      <c r="H34" s="104"/>
+      <c r="I34" s="104"/>
+      <c r="J34" s="104"/>
+      <c r="K34" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="L34" s="68"/>
+      <c r="L34" s="62"/>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B35" s="105"/>
-      <c r="C35" s="101"/>
-      <c r="D35" s="101"/>
-      <c r="E35" s="101"/>
-      <c r="F35" s="56"/>
-      <c r="G35" s="56"/>
-      <c r="H35" s="56"/>
-      <c r="I35" s="56"/>
-      <c r="J35" s="56"/>
-      <c r="K35" s="56" t="s">
+      <c r="B35" s="116"/>
+      <c r="C35" s="104"/>
+      <c r="D35" s="104"/>
+      <c r="E35" s="104"/>
+      <c r="F35" s="104"/>
+      <c r="G35" s="104"/>
+      <c r="H35" s="104"/>
+      <c r="I35" s="104"/>
+      <c r="J35" s="104"/>
+      <c r="K35" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="L35" s="68"/>
+      <c r="L35" s="62"/>
     </row>
     <row r="36" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="106"/>
-      <c r="C36" s="102"/>
-      <c r="D36" s="102"/>
-      <c r="E36" s="102"/>
-      <c r="F36" s="57"/>
-      <c r="G36" s="57"/>
-      <c r="H36" s="57"/>
-      <c r="I36" s="57"/>
-      <c r="J36" s="57"/>
-      <c r="K36" s="57" t="s">
+      <c r="B36" s="117"/>
+      <c r="C36" s="105"/>
+      <c r="D36" s="105"/>
+      <c r="E36" s="105"/>
+      <c r="F36" s="105"/>
+      <c r="G36" s="105"/>
+      <c r="H36" s="105"/>
+      <c r="I36" s="105"/>
+      <c r="J36" s="105"/>
+      <c r="K36" s="82" t="s">
         <v>29</v>
       </c>
-      <c r="L36" s="69"/>
+      <c r="L36" s="63"/>
     </row>
     <row r="38" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="2:12" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B39" s="125" t="s">
+      <c r="B39" s="133" t="s">
         <v>31</v>
       </c>
-      <c r="C39" s="126"/>
-      <c r="D39" s="126"/>
-      <c r="E39" s="126"/>
-      <c r="F39" s="126"/>
-      <c r="G39" s="126"/>
-      <c r="H39" s="126"/>
-      <c r="I39" s="126"/>
-      <c r="J39" s="126"/>
-      <c r="K39" s="126"/>
-      <c r="L39" s="127"/>
+      <c r="C39" s="134"/>
+      <c r="D39" s="134"/>
+      <c r="E39" s="134"/>
+      <c r="F39" s="134"/>
+      <c r="G39" s="134"/>
+      <c r="H39" s="134"/>
+      <c r="I39" s="134"/>
+      <c r="J39" s="134"/>
+      <c r="K39" s="134"/>
+      <c r="L39" s="135"/>
     </row>
     <row r="40" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="2:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D41" s="122" t="s">
-        <v>55</v>
-      </c>
-      <c r="E41" s="123"/>
-      <c r="F41" s="123"/>
-      <c r="G41" s="123"/>
-      <c r="H41" s="123"/>
-      <c r="I41" s="123"/>
-      <c r="J41" s="124"/>
+      <c r="D41" s="130" t="s">
+        <v>53</v>
+      </c>
+      <c r="E41" s="131"/>
+      <c r="F41" s="131"/>
+      <c r="G41" s="131"/>
+      <c r="H41" s="131"/>
+      <c r="I41" s="131"/>
+      <c r="J41" s="132"/>
     </row>
     <row r="42" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D43" s="65" t="s">
+      <c r="D43" s="59" t="s">
         <v>33</v>
       </c>
       <c r="E43" s="52" t="s">
@@ -5232,368 +5441,368 @@
         <v>47</v>
       </c>
       <c r="G43" s="52" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H43" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="I43" s="66" t="s">
-        <v>53</v>
-      </c>
-      <c r="J43" s="73" t="s">
-        <v>64</v>
+      <c r="I43" s="60" t="s">
+        <v>51</v>
+      </c>
+      <c r="J43" s="67" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D44" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="E44" s="97" t="s">
-        <v>52</v>
+      <c r="E44" s="118" t="s">
+        <v>50</v>
       </c>
       <c r="F44" s="41" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G44" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="H44" s="97">
+        <v>81</v>
+      </c>
+      <c r="H44" s="118">
         <v>40</v>
       </c>
       <c r="I44" s="41">
         <v>100</v>
       </c>
-      <c r="J44" s="71" t="s">
-        <v>65</v>
+      <c r="J44" s="65" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D45" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="E45" s="98"/>
+      <c r="E45" s="119"/>
       <c r="F45" s="51" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G45" s="51" t="s">
-        <v>82</v>
-      </c>
-      <c r="H45" s="98"/>
+        <v>80</v>
+      </c>
+      <c r="H45" s="119"/>
       <c r="I45" s="51">
         <v>127</v>
       </c>
-      <c r="J45" s="72" t="s">
-        <v>66</v>
+      <c r="J45" s="66" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D46" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="E46" s="98"/>
+      <c r="E46" s="119"/>
       <c r="F46" s="51" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G46" s="51" t="s">
-        <v>81</v>
-      </c>
-      <c r="H46" s="98"/>
+        <v>79</v>
+      </c>
+      <c r="H46" s="119"/>
       <c r="I46" s="51">
         <v>100</v>
       </c>
       <c r="J46" s="49" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D47" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="E47" s="99"/>
+      <c r="E47" s="120"/>
       <c r="F47" s="51" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G47" s="51" t="s">
-        <v>80</v>
-      </c>
-      <c r="H47" s="99"/>
+        <v>78</v>
+      </c>
+      <c r="H47" s="120"/>
       <c r="I47" s="51">
         <v>100</v>
       </c>
       <c r="J47" s="49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D48" s="64" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" s="121" t="s">
+        <v>50</v>
+      </c>
+      <c r="F48" s="64" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D48" s="70" t="s">
+      <c r="G48" s="64" t="s">
+        <v>82</v>
+      </c>
+      <c r="H48" s="121">
+        <v>60</v>
+      </c>
+      <c r="I48" s="64">
+        <v>225</v>
+      </c>
+      <c r="J48" s="49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D49" s="64" t="s">
+        <v>21</v>
+      </c>
+      <c r="E49" s="122"/>
+      <c r="F49" s="64" t="s">
+        <v>66</v>
+      </c>
+      <c r="G49" s="64" t="s">
+        <v>83</v>
+      </c>
+      <c r="H49" s="122"/>
+      <c r="I49" s="64">
+        <v>263</v>
+      </c>
+      <c r="J49" s="66" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D50" s="64" t="s">
+        <v>20</v>
+      </c>
+      <c r="E50" s="122"/>
+      <c r="F50" s="64" t="s">
+        <v>67</v>
+      </c>
+      <c r="G50" s="64" t="s">
+        <v>84</v>
+      </c>
+      <c r="H50" s="122"/>
+      <c r="I50" s="64">
+        <v>225</v>
+      </c>
+      <c r="J50" s="49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D51" s="64" t="s">
+        <v>38</v>
+      </c>
+      <c r="E51" s="123"/>
+      <c r="F51" s="64" t="s">
+        <v>68</v>
+      </c>
+      <c r="G51" s="64" t="s">
+        <v>85</v>
+      </c>
+      <c r="H51" s="123"/>
+      <c r="I51" s="64">
+        <v>225</v>
+      </c>
+      <c r="J51" s="49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D52" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="E48" s="94" t="s">
-        <v>52</v>
-      </c>
-      <c r="F48" s="70" t="s">
-        <v>67</v>
-      </c>
-      <c r="G48" s="70" t="s">
-        <v>84</v>
-      </c>
-      <c r="H48" s="94">
-        <v>60</v>
-      </c>
-      <c r="I48" s="70">
-        <v>225</v>
-      </c>
-      <c r="J48" s="49" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D49" s="70" t="s">
+      <c r="E52" s="124" t="s">
+        <v>50</v>
+      </c>
+      <c r="F52" s="58" t="s">
+        <v>69</v>
+      </c>
+      <c r="G52" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="H52" s="124">
+        <v>80</v>
+      </c>
+      <c r="I52" s="58">
+        <v>400</v>
+      </c>
+      <c r="J52" s="49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D53" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="E49" s="95"/>
-      <c r="F49" s="70" t="s">
-        <v>68</v>
-      </c>
-      <c r="G49" s="70" t="s">
-        <v>85</v>
-      </c>
-      <c r="H49" s="95"/>
-      <c r="I49" s="70">
-        <v>263</v>
-      </c>
-      <c r="J49" s="72" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D50" s="70" t="s">
+      <c r="E53" s="125"/>
+      <c r="F53" s="58" t="s">
+        <v>70</v>
+      </c>
+      <c r="G53" s="58" t="s">
+        <v>88</v>
+      </c>
+      <c r="H53" s="125"/>
+      <c r="I53" s="58">
+        <v>457</v>
+      </c>
+      <c r="J53" s="66" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D54" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="E50" s="95"/>
-      <c r="F50" s="70" t="s">
-        <v>69</v>
-      </c>
-      <c r="G50" s="70" t="s">
+      <c r="E54" s="125"/>
+      <c r="F54" s="58" t="s">
+        <v>71</v>
+      </c>
+      <c r="G54" s="58" t="s">
+        <v>87</v>
+      </c>
+      <c r="H54" s="125"/>
+      <c r="I54" s="58">
+        <v>400</v>
+      </c>
+      <c r="J54" s="49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D55" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="E55" s="126"/>
+      <c r="F55" s="58" t="s">
+        <v>72</v>
+      </c>
+      <c r="G55" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="H50" s="95"/>
-      <c r="I50" s="70">
-        <v>225</v>
-      </c>
-      <c r="J50" s="49" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D51" s="70" t="s">
+      <c r="H55" s="126"/>
+      <c r="I55" s="58">
+        <v>400</v>
+      </c>
+      <c r="J55" s="49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D56" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="E56" s="127" t="s">
+        <v>50</v>
+      </c>
+      <c r="F56" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="G56" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="H56" s="127">
+        <v>100</v>
+      </c>
+      <c r="I56" s="57">
+        <v>625</v>
+      </c>
+      <c r="J56" s="49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D57" s="57" t="s">
+        <v>21</v>
+      </c>
+      <c r="E57" s="128"/>
+      <c r="F57" s="57" t="s">
+        <v>93</v>
+      </c>
+      <c r="G57" s="57" t="s">
+        <v>74</v>
+      </c>
+      <c r="H57" s="128"/>
+      <c r="I57" s="57">
+        <v>645</v>
+      </c>
+      <c r="J57" s="66" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D58" s="57" t="s">
+        <v>20</v>
+      </c>
+      <c r="E58" s="128"/>
+      <c r="F58" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="G58" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="H58" s="128"/>
+      <c r="I58" s="57">
+        <v>625</v>
+      </c>
+      <c r="J58" s="49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="59" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D59" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="E51" s="96"/>
-      <c r="F51" s="70" t="s">
-        <v>70</v>
-      </c>
-      <c r="G51" s="70" t="s">
-        <v>87</v>
-      </c>
-      <c r="H51" s="96"/>
-      <c r="I51" s="70">
-        <v>225</v>
-      </c>
-      <c r="J51" s="49" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D52" s="64" t="s">
-        <v>19</v>
-      </c>
-      <c r="E52" s="107" t="s">
-        <v>52</v>
-      </c>
-      <c r="F52" s="64" t="s">
-        <v>71</v>
-      </c>
-      <c r="G52" s="64" t="s">
-        <v>91</v>
-      </c>
-      <c r="H52" s="107">
-        <v>80</v>
-      </c>
-      <c r="I52" s="64">
-        <v>400</v>
-      </c>
-      <c r="J52" s="49" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D53" s="64" t="s">
-        <v>21</v>
-      </c>
-      <c r="E53" s="108"/>
-      <c r="F53" s="64" t="s">
-        <v>72</v>
-      </c>
-      <c r="G53" s="64" t="s">
-        <v>90</v>
-      </c>
-      <c r="H53" s="108"/>
-      <c r="I53" s="64">
-        <v>457</v>
-      </c>
-      <c r="J53" s="72" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D54" s="64" t="s">
-        <v>20</v>
-      </c>
-      <c r="E54" s="108"/>
-      <c r="F54" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="G54" s="64" t="s">
-        <v>89</v>
-      </c>
-      <c r="H54" s="108"/>
-      <c r="I54" s="64">
-        <v>400</v>
-      </c>
-      <c r="J54" s="49" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D55" s="64" t="s">
-        <v>38</v>
-      </c>
-      <c r="E55" s="109"/>
-      <c r="F55" s="64" t="s">
-        <v>74</v>
-      </c>
-      <c r="G55" s="64" t="s">
-        <v>88</v>
-      </c>
-      <c r="H55" s="109"/>
-      <c r="I55" s="64">
-        <v>400</v>
-      </c>
-      <c r="J55" s="49" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D56" s="63" t="s">
-        <v>19</v>
-      </c>
-      <c r="E56" s="110" t="s">
-        <v>52</v>
-      </c>
-      <c r="F56" s="63" t="s">
-        <v>75</v>
-      </c>
-      <c r="G56" s="63" t="s">
-        <v>75</v>
-      </c>
-      <c r="H56" s="110">
-        <v>100</v>
-      </c>
-      <c r="I56" s="63">
+      <c r="E59" s="129"/>
+      <c r="F59" s="61" t="s">
+        <v>95</v>
+      </c>
+      <c r="G59" s="61" t="s">
+        <v>76</v>
+      </c>
+      <c r="H59" s="129"/>
+      <c r="I59" s="61">
         <v>625</v>
       </c>
-      <c r="J56" s="49" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D57" s="63" t="s">
-        <v>21</v>
-      </c>
-      <c r="E57" s="111"/>
-      <c r="F57" s="63" t="s">
-        <v>76</v>
-      </c>
-      <c r="G57" s="63" t="s">
-        <v>76</v>
-      </c>
-      <c r="H57" s="111"/>
-      <c r="I57" s="63">
-        <v>645</v>
-      </c>
-      <c r="J57" s="72" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D58" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="E58" s="111"/>
-      <c r="F58" s="63" t="s">
-        <v>77</v>
-      </c>
-      <c r="G58" s="63" t="s">
-        <v>77</v>
-      </c>
-      <c r="H58" s="111"/>
-      <c r="I58" s="63">
-        <v>625</v>
-      </c>
-      <c r="J58" s="49" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="59" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D59" s="67" t="s">
-        <v>38</v>
-      </c>
-      <c r="E59" s="112"/>
-      <c r="F59" s="67" t="s">
-        <v>78</v>
-      </c>
-      <c r="G59" s="67" t="s">
-        <v>78</v>
-      </c>
-      <c r="H59" s="112"/>
-      <c r="I59" s="67">
-        <v>625</v>
-      </c>
       <c r="J59" s="50" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="61" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="62" spans="2:12" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B62" s="128" t="s">
+      <c r="B62" s="109" t="s">
         <v>37</v>
       </c>
-      <c r="C62" s="129"/>
-      <c r="D62" s="129"/>
-      <c r="E62" s="129"/>
-      <c r="F62" s="129"/>
-      <c r="G62" s="129"/>
-      <c r="H62" s="129"/>
-      <c r="I62" s="129"/>
-      <c r="J62" s="129"/>
-      <c r="K62" s="129"/>
-      <c r="L62" s="130"/>
+      <c r="C62" s="110"/>
+      <c r="D62" s="110"/>
+      <c r="E62" s="110"/>
+      <c r="F62" s="110"/>
+      <c r="G62" s="110"/>
+      <c r="H62" s="110"/>
+      <c r="I62" s="110"/>
+      <c r="J62" s="110"/>
+      <c r="K62" s="110"/>
+      <c r="L62" s="111"/>
     </row>
     <row r="63" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="64" spans="2:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D64" s="119" t="s">
-        <v>48</v>
-      </c>
-      <c r="E64" s="120"/>
-      <c r="F64" s="120"/>
-      <c r="G64" s="120"/>
-      <c r="H64" s="120"/>
-      <c r="I64" s="120"/>
-      <c r="J64" s="121"/>
-    </row>
-    <row r="65" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="66" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D64" s="106" t="s">
+        <v>97</v>
+      </c>
+      <c r="E64" s="107"/>
+      <c r="F64" s="107"/>
+      <c r="G64" s="107"/>
+      <c r="H64" s="107"/>
+      <c r="I64" s="107"/>
+      <c r="J64" s="108"/>
+    </row>
+    <row r="65" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E66" s="46" t="s">
         <v>45</v>
       </c>
@@ -5601,7 +5810,7 @@
         <v>46</v>
       </c>
       <c r="G66" s="47" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H66" s="47" t="s">
         <v>43</v>
@@ -5610,285 +5819,350 @@
         <v>42</v>
       </c>
     </row>
-    <row r="67" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="E67" s="44">
+    <row r="67" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E67" s="70">
         <v>4</v>
       </c>
-      <c r="F67" s="116" t="s">
-        <v>54</v>
-      </c>
-      <c r="G67" s="116" t="s">
+      <c r="F67" s="112" t="s">
+        <v>52</v>
+      </c>
+      <c r="G67" s="112" t="s">
         <v>39</v>
       </c>
-      <c r="H67" s="116">
+      <c r="H67" s="112">
         <v>0</v>
       </c>
-      <c r="I67" s="45">
+      <c r="I67" s="71">
         <v>35</v>
       </c>
     </row>
-    <row r="68" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E68" s="42">
         <v>8</v>
       </c>
-      <c r="F68" s="117"/>
-      <c r="G68" s="117"/>
-      <c r="H68" s="117"/>
+      <c r="F68" s="113"/>
+      <c r="G68" s="113"/>
+      <c r="H68" s="113"/>
       <c r="I68" s="43">
         <v>1351</v>
       </c>
     </row>
-    <row r="69" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E69" s="42">
         <v>12</v>
       </c>
-      <c r="F69" s="117"/>
-      <c r="G69" s="117"/>
-      <c r="H69" s="117"/>
+      <c r="F69" s="113"/>
+      <c r="G69" s="113"/>
+      <c r="H69" s="113"/>
       <c r="I69" s="43">
         <v>61347</v>
       </c>
     </row>
-    <row r="70" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E70" s="42">
         <v>16</v>
       </c>
-      <c r="F70" s="117"/>
-      <c r="G70" s="117"/>
-      <c r="H70" s="117"/>
+      <c r="F70" s="113"/>
+      <c r="G70" s="113"/>
+      <c r="H70" s="113"/>
       <c r="I70" s="43">
         <v>3039751</v>
       </c>
     </row>
-    <row r="71" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E71" s="42">
         <v>20</v>
       </c>
-      <c r="F71" s="118"/>
-      <c r="G71" s="118"/>
-      <c r="H71" s="118"/>
+      <c r="F71" s="114"/>
+      <c r="G71" s="114"/>
+      <c r="H71" s="114"/>
       <c r="I71" s="43">
         <v>98795020</v>
       </c>
     </row>
-    <row r="72" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="E72" s="59">
+    <row r="72" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E72" s="53">
         <v>4</v>
       </c>
-      <c r="F72" s="113" t="s">
-        <v>54</v>
-      </c>
-      <c r="G72" s="113" t="s">
+      <c r="F72" s="145" t="s">
+        <v>52</v>
+      </c>
+      <c r="G72" s="145" t="s">
         <v>39</v>
       </c>
-      <c r="H72" s="113" t="s">
+      <c r="H72" s="145" t="s">
         <v>44</v>
       </c>
-      <c r="I72" s="60">
+      <c r="I72" s="54">
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="E73" s="59">
+    <row r="73" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E73" s="53">
         <v>8</v>
       </c>
-      <c r="F73" s="114"/>
-      <c r="G73" s="114"/>
-      <c r="H73" s="114"/>
-      <c r="I73" s="60">
+      <c r="F73" s="145"/>
+      <c r="G73" s="145"/>
+      <c r="H73" s="145"/>
+      <c r="I73" s="54">
         <v>650</v>
       </c>
     </row>
-    <row r="74" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="E74" s="59">
+    <row r="74" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E74" s="53">
         <v>12</v>
       </c>
-      <c r="F74" s="114"/>
-      <c r="G74" s="114"/>
-      <c r="H74" s="114"/>
-      <c r="I74" s="60">
+      <c r="F74" s="145"/>
+      <c r="G74" s="145"/>
+      <c r="H74" s="145"/>
+      <c r="I74" s="54">
         <v>22589</v>
       </c>
     </row>
-    <row r="75" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="E75" s="59">
+    <row r="75" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E75" s="53">
         <v>16</v>
       </c>
-      <c r="F75" s="114"/>
-      <c r="G75" s="114"/>
-      <c r="H75" s="114"/>
-      <c r="I75" s="60">
+      <c r="F75" s="145"/>
+      <c r="G75" s="145"/>
+      <c r="H75" s="145"/>
+      <c r="I75" s="54">
         <v>840947</v>
       </c>
     </row>
-    <row r="76" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E76" s="61">
+    <row r="76" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E76" s="53">
         <v>20</v>
       </c>
-      <c r="F76" s="115"/>
-      <c r="G76" s="115"/>
-      <c r="H76" s="115"/>
-      <c r="I76" s="62">
+      <c r="F76" s="145"/>
+      <c r="G76" s="145"/>
+      <c r="H76" s="145"/>
+      <c r="I76" s="54">
         <v>37258591</v>
       </c>
     </row>
-    <row r="77" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="E77" s="33"/>
-    </row>
-    <row r="78" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="79" spans="4:10" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D79" s="119" t="s">
+    <row r="77" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E77" s="72">
+        <v>4</v>
+      </c>
+      <c r="F77" s="101" t="s">
+        <v>91</v>
+      </c>
+      <c r="G77" s="101"/>
+      <c r="H77" s="101"/>
+      <c r="I77" s="73">
+        <f>POWER(2.5,E77)</f>
+        <v>39.0625</v>
+      </c>
+    </row>
+    <row r="78" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E78" s="74">
+        <v>8</v>
+      </c>
+      <c r="F78" s="101"/>
+      <c r="G78" s="101"/>
+      <c r="H78" s="101"/>
+      <c r="I78" s="73">
+        <f t="shared" ref="I78:I81" si="0">POWER(2.5,E78)</f>
+        <v>1525.87890625</v>
+      </c>
+    </row>
+    <row r="79" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E79" s="74">
+        <v>12</v>
+      </c>
+      <c r="F79" s="101"/>
+      <c r="G79" s="101"/>
+      <c r="H79" s="101"/>
+      <c r="I79" s="73">
+        <f t="shared" si="0"/>
+        <v>59604.644775390625</v>
+      </c>
+    </row>
+    <row r="80" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E80" s="74">
+        <v>16</v>
+      </c>
+      <c r="F80" s="101"/>
+      <c r="G80" s="101"/>
+      <c r="H80" s="101"/>
+      <c r="I80" s="73">
+        <f t="shared" si="0"/>
+        <v>2328306.4365386963</v>
+      </c>
+    </row>
+    <row r="81" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E81" s="75">
+        <v>20</v>
+      </c>
+      <c r="F81" s="102"/>
+      <c r="G81" s="102"/>
+      <c r="H81" s="102"/>
+      <c r="I81" s="76">
+        <f t="shared" si="0"/>
+        <v>90949470.177292824</v>
+      </c>
+    </row>
+    <row r="82" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="E82" s="33"/>
+    </row>
+    <row r="83" spans="4:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E83" s="33"/>
+    </row>
+    <row r="84" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="85" spans="4:10" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D85" s="106" t="s">
+        <v>98</v>
+      </c>
+      <c r="E85" s="107"/>
+      <c r="F85" s="107"/>
+      <c r="G85" s="107"/>
+      <c r="H85" s="107"/>
+      <c r="I85" s="107"/>
+      <c r="J85" s="108"/>
+    </row>
+    <row r="86" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="87" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E87" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="F87" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="G87" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="H87" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="I87" s="48" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="88" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="E88" s="44">
+        <v>4</v>
+      </c>
+      <c r="F88" s="112" t="s">
+        <v>57</v>
+      </c>
+      <c r="G88" s="112" t="s">
+        <v>44</v>
+      </c>
+      <c r="H88" s="112" t="s">
+        <v>39</v>
+      </c>
+      <c r="I88" s="45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="89" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="E89" s="42">
+        <v>8</v>
+      </c>
+      <c r="F89" s="113"/>
+      <c r="G89" s="113"/>
+      <c r="H89" s="113"/>
+      <c r="I89" s="43">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="90" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="E90" s="42">
+        <v>12</v>
+      </c>
+      <c r="F90" s="113"/>
+      <c r="G90" s="113"/>
+      <c r="H90" s="113"/>
+      <c r="I90" s="43">
+        <v>23080</v>
+      </c>
+    </row>
+    <row r="91" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="E91" s="42">
+        <v>16</v>
+      </c>
+      <c r="F91" s="113"/>
+      <c r="G91" s="113"/>
+      <c r="H91" s="113"/>
+      <c r="I91" s="43">
+        <v>747081</v>
+      </c>
+    </row>
+    <row r="92" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="E92" s="42">
+        <v>20</v>
+      </c>
+      <c r="F92" s="114"/>
+      <c r="G92" s="114"/>
+      <c r="H92" s="114"/>
+      <c r="I92" s="43">
+        <v>34214860</v>
+      </c>
+    </row>
+    <row r="93" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="E93" s="53">
+        <v>4</v>
+      </c>
+      <c r="F93" s="136" t="s">
+        <v>57</v>
+      </c>
+      <c r="G93" s="136" t="s">
+        <v>44</v>
+      </c>
+      <c r="H93" s="136" t="s">
         <v>49</v>
       </c>
-      <c r="E79" s="120"/>
-      <c r="F79" s="120"/>
-      <c r="G79" s="120"/>
-      <c r="H79" s="120"/>
-      <c r="I79" s="120"/>
-      <c r="J79" s="121"/>
-    </row>
-    <row r="80" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="81" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E81" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="F81" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="G81" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="H81" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="I81" s="48" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="82" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E82" s="44">
+      <c r="I93" s="54">
         <v>4</v>
       </c>
-      <c r="F82" s="116" t="s">
-        <v>59</v>
-      </c>
-      <c r="G82" s="116" t="s">
-        <v>44</v>
-      </c>
-      <c r="H82" s="116" t="s">
-        <v>39</v>
-      </c>
-      <c r="I82" s="45">
+    </row>
+    <row r="94" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="E94" s="53">
+        <v>8</v>
+      </c>
+      <c r="F94" s="137"/>
+      <c r="G94" s="137"/>
+      <c r="H94" s="137"/>
+      <c r="I94" s="54">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="95" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="E95" s="53">
+        <v>12</v>
+      </c>
+      <c r="F95" s="137"/>
+      <c r="G95" s="137"/>
+      <c r="H95" s="137"/>
+      <c r="I95" s="54">
+        <v>22283</v>
+      </c>
+    </row>
+    <row r="96" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="E96" s="53">
+        <v>16</v>
+      </c>
+      <c r="F96" s="137"/>
+      <c r="G96" s="137"/>
+      <c r="H96" s="137"/>
+      <c r="I96" s="54">
+        <v>761323</v>
+      </c>
+    </row>
+    <row r="97" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E97" s="55">
         <v>20</v>
       </c>
-    </row>
-    <row r="83" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E83" s="42">
-        <v>8</v>
-      </c>
-      <c r="F83" s="117"/>
-      <c r="G83" s="117"/>
-      <c r="H83" s="117"/>
-      <c r="I83" s="43">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="84" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E84" s="42">
-        <v>12</v>
-      </c>
-      <c r="F84" s="117"/>
-      <c r="G84" s="117"/>
-      <c r="H84" s="117"/>
-      <c r="I84" s="43">
-        <v>23080</v>
-      </c>
-    </row>
-    <row r="85" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E85" s="42">
-        <v>16</v>
-      </c>
-      <c r="F85" s="117"/>
-      <c r="G85" s="117"/>
-      <c r="H85" s="117"/>
-      <c r="I85" s="43">
-        <v>747081</v>
-      </c>
-    </row>
-    <row r="86" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E86" s="42">
-        <v>20</v>
-      </c>
-      <c r="F86" s="118"/>
-      <c r="G86" s="118"/>
-      <c r="H86" s="118"/>
-      <c r="I86" s="43">
-        <v>34214860</v>
-      </c>
-    </row>
-    <row r="87" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E87" s="59">
-        <v>4</v>
-      </c>
-      <c r="F87" s="113" t="s">
-        <v>59</v>
-      </c>
-      <c r="G87" s="113" t="s">
-        <v>44</v>
-      </c>
-      <c r="H87" s="113" t="s">
-        <v>51</v>
-      </c>
-      <c r="I87" s="60">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="88" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E88" s="59">
-        <v>8</v>
-      </c>
-      <c r="F88" s="114"/>
-      <c r="G88" s="114"/>
-      <c r="H88" s="114"/>
-      <c r="I88" s="60">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="89" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E89" s="59">
-        <v>12</v>
-      </c>
-      <c r="F89" s="114"/>
-      <c r="G89" s="114"/>
-      <c r="H89" s="114"/>
-      <c r="I89" s="60">
-        <v>22283</v>
-      </c>
-    </row>
-    <row r="90" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E90" s="59">
-        <v>16</v>
-      </c>
-      <c r="F90" s="114"/>
-      <c r="G90" s="114"/>
-      <c r="H90" s="114"/>
-      <c r="I90" s="60">
-        <v>761323</v>
-      </c>
-    </row>
-    <row r="91" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E91" s="61">
-        <v>20</v>
-      </c>
-      <c r="F91" s="115"/>
-      <c r="G91" s="115"/>
-      <c r="H91" s="115"/>
-      <c r="I91" s="62">
+      <c r="F97" s="138"/>
+      <c r="G97" s="138"/>
+      <c r="H97" s="138"/>
+      <c r="I97" s="56">
         <v>38700837</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="45">
     <mergeCell ref="D4:J4"/>
     <mergeCell ref="B2:L2"/>
     <mergeCell ref="H67:H71"/>
@@ -5897,14 +6171,15 @@
     <mergeCell ref="H52:H55"/>
     <mergeCell ref="G72:G76"/>
     <mergeCell ref="H72:H76"/>
-    <mergeCell ref="F87:F91"/>
-    <mergeCell ref="G87:G91"/>
-    <mergeCell ref="F82:F86"/>
-    <mergeCell ref="G82:G86"/>
-    <mergeCell ref="H87:H91"/>
-    <mergeCell ref="H82:H86"/>
     <mergeCell ref="D64:J64"/>
-    <mergeCell ref="D79:J79"/>
+    <mergeCell ref="K7:K29"/>
+    <mergeCell ref="F93:F97"/>
+    <mergeCell ref="G93:G97"/>
+    <mergeCell ref="F88:F92"/>
+    <mergeCell ref="G88:G92"/>
+    <mergeCell ref="H93:H97"/>
+    <mergeCell ref="H88:H92"/>
+    <mergeCell ref="D85:J85"/>
     <mergeCell ref="B62:L62"/>
     <mergeCell ref="F67:F71"/>
     <mergeCell ref="G67:G71"/>
@@ -5920,9 +6195,75 @@
     <mergeCell ref="D7:D36"/>
     <mergeCell ref="C7:C36"/>
     <mergeCell ref="E12:E36"/>
+    <mergeCell ref="F77:F81"/>
+    <mergeCell ref="G77:G81"/>
+    <mergeCell ref="H77:H81"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="J30:J36"/>
+    <mergeCell ref="I27:I36"/>
+    <mergeCell ref="H25:H36"/>
+    <mergeCell ref="G21:G36"/>
+    <mergeCell ref="F17:F36"/>
+    <mergeCell ref="G7:G16"/>
+    <mergeCell ref="H7:H20"/>
+    <mergeCell ref="I7:I24"/>
+    <mergeCell ref="J7:J26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{109DB7DB-D99C-41F8-9D21-DE922C38A101}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="47" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>